<commit_message>
cambios de estructura, listas de líneas de absorción
</commit_message>
<xml_diff>
--- a/Scripts/Growth_curve/lines.xlsx
+++ b/Scripts/Growth_curve/lines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Documents\Semestre8y9\Trabajo_grado\Scripts\Growth_curve\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Documents\Semestre8y9\Trabajo_grado\Tesis_Estrellas_binarias\Scripts\Growth_curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE53BAE-8473-4A68-8400-485E57E9DEE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DF2FCC-B88E-4468-B0F9-EA66A6CC1FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="1000" activeTab="3" xr2:uid="{F6AB02B0-D3FC-4D31-BBAC-19215CAECE6C}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="34">
   <si>
     <t>wavelenght</t>
   </si>
@@ -130,16 +130,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>waveobs</t>
-  </si>
-  <si>
-    <t>Fe 1</t>
-  </si>
-  <si>
-    <t>Fe 2</t>
-  </si>
-  <si>
-    <t>Ti 2</t>
+    <t>wave_peak</t>
   </si>
 </sst>
 </file>
@@ -10604,1574 +10595,1257 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE75F030-7D08-4563-BE0C-CE0E8301EC84}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="G1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+    <row r="2" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="8">
         <v>3761.32</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2">
+      <c r="H2">
         <v>3760.75</v>
       </c>
-      <c r="D2">
+      <c r="I2">
         <v>3762.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="8">
         <v>3763.79</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3">
+      <c r="H3">
         <v>3763.4</v>
       </c>
-      <c r="D3">
+      <c r="I3">
         <v>3764.34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+    <row r="4" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="8">
         <v>3767.19</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4">
+      <c r="H4">
         <v>3766.7</v>
       </c>
-      <c r="D4">
+      <c r="I4">
         <v>3767.55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+    <row r="5" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="8">
         <v>3769.46</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <f>A5-0.05</f>
+      <c r="H5">
+        <f>G5-0.05</f>
         <v>3769.41</v>
       </c>
-      <c r="D5">
-        <f>A5+0.05</f>
+      <c r="I5">
+        <f>G5+0.05</f>
         <v>3769.51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+    <row r="6" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="8">
         <v>3770.63</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ref="C6:C7" si="0">A6-0.05</f>
+      <c r="H6">
+        <f>G6-0.05</f>
         <v>3770.58</v>
       </c>
-      <c r="D6">
-        <f t="shared" ref="D6:D7" si="1">A6+0.05</f>
+      <c r="I6">
+        <f>G6+0.05</f>
         <v>3770.6800000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="8">
         <v>3774.33</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
+      <c r="H7">
+        <f>G7-0.05</f>
         <v>3774.2799999999997</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
+      <c r="I7">
+        <f>G7+0.05</f>
         <v>3774.38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="8">
         <v>3783.35</v>
       </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8">
+      <c r="H8">
         <v>3783.25</v>
       </c>
-      <c r="D8">
+      <c r="I8">
         <v>3783.75</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+    <row r="9" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="8">
         <v>3787.88</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9">
+      <c r="H9">
         <v>3787.58</v>
       </c>
-      <c r="D9">
+      <c r="I9">
         <v>3788.21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+    <row r="10" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="8">
         <v>3788.7</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
-        <f>A10-0.05</f>
+      <c r="H10">
+        <f>G10-0.05</f>
         <v>3788.6499999999996</v>
       </c>
-      <c r="D10">
-        <f>A10+0.05</f>
+      <c r="I10">
+        <f>G10+0.05</f>
         <v>3788.75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+    <row r="11" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="10">
         <v>3795</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11">
+      <c r="H11">
         <v>3794.58</v>
       </c>
-      <c r="D11">
+      <c r="I11">
         <v>3795.38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+    <row r="12" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="8">
         <v>3797.9</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <f>A12-0.05</f>
+      <c r="H12">
+        <f>G12-0.05</f>
         <v>3797.85</v>
       </c>
-      <c r="D12">
-        <f>A12+0.05</f>
+      <c r="I12">
+        <f>G12+0.05</f>
         <v>3797.9500000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+    <row r="13" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="8">
         <v>3814.58</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13">
+      <c r="H13">
         <v>3814.18</v>
       </c>
-      <c r="D13">
+      <c r="I13">
         <v>3815.1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+    <row r="14" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G14" s="8">
         <v>3815.84</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14">
+      <c r="H14">
         <v>3815.5</v>
       </c>
-      <c r="D14">
+      <c r="I14">
         <v>3816.3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+    <row r="15" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="8">
         <v>3820.43</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="18">
+      <c r="H15" s="18">
         <v>3819.98</v>
       </c>
-      <c r="D15">
+      <c r="I15">
         <v>3821.02</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+    <row r="16" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="8">
         <v>3824.45</v>
       </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16">
+      <c r="H16">
         <v>3824.05</v>
       </c>
-      <c r="D16">
+      <c r="I16">
         <v>3824.91</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="8">
         <v>3825.88</v>
       </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17">
+      <c r="H17">
         <v>3825.5</v>
       </c>
-      <c r="D17">
+      <c r="I17">
         <v>3826.46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="8">
         <v>3827.83</v>
       </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18">
+      <c r="H18">
         <v>3827.43</v>
       </c>
-      <c r="D18">
+      <c r="I18">
         <v>3828.23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="8">
         <v>3829.35</v>
       </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19">
-        <f>A19-0.05</f>
+      <c r="H19">
+        <f>G19-0.05</f>
         <v>3829.2999999999997</v>
       </c>
-      <c r="D19">
-        <f>A19+0.05</f>
+      <c r="I19">
+        <f>G19+0.05</f>
         <v>3829.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="8">
         <v>3832.3</v>
       </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20">
-        <f>A20-0.05</f>
+      <c r="H20">
+        <f>G20-0.05</f>
         <v>3832.25</v>
       </c>
-      <c r="D20">
-        <f>A20+0.05</f>
+      <c r="I20">
+        <f>G20+0.05</f>
         <v>3832.3500000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="8">
         <v>3834.23</v>
       </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21">
+      <c r="H21">
         <v>3833.77</v>
       </c>
-      <c r="D21">
+      <c r="I21">
         <v>3834.69</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="8">
         <v>3835.39</v>
       </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <f>A22-0.05</f>
+      <c r="H22">
+        <f>G22-0.05</f>
         <v>3835.3399999999997</v>
       </c>
-      <c r="D22">
-        <f>A22+0.05</f>
+      <c r="I22">
+        <f>G22+0.05</f>
         <v>3835.44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="8">
         <v>3838.29</v>
       </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23">
-        <f>A23-0.05</f>
+      <c r="H23">
+        <f>G23-0.05</f>
         <v>3838.24</v>
       </c>
-      <c r="D23">
-        <f>A23+0.05</f>
+      <c r="I23">
+        <f>G23+0.05</f>
         <v>3838.34</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="8">
         <v>3843.03</v>
       </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24">
-        <f>A24-0.05</f>
+      <c r="H24">
+        <f>G24-0.05</f>
         <v>3842.98</v>
       </c>
-      <c r="D24">
-        <f>A24+0.05</f>
+      <c r="I24">
+        <f>G24+0.05</f>
         <v>3843.0800000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="10">
         <v>3850</v>
       </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25">
+      <c r="H25">
         <v>3849.65</v>
       </c>
-      <c r="D25">
+      <c r="I25">
         <v>3850.3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="8">
         <v>3850.82</v>
       </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26">
+      <c r="H26">
         <v>3850.55</v>
       </c>
-      <c r="D26">
+      <c r="I26">
         <v>3851.15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+    <row r="27" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="8">
         <v>3856.37</v>
       </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27">
+      <c r="H27">
         <v>3855.97</v>
       </c>
-      <c r="D27">
+      <c r="I27">
         <v>3856.85</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+    <row r="28" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="8">
         <v>3858.3</v>
       </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28">
-        <f>A28-0.05</f>
+      <c r="H28">
+        <f>G28-0.05</f>
         <v>3858.25</v>
       </c>
-      <c r="D28">
-        <f>A28+0.05</f>
+      <c r="I28">
+        <f>G28+0.05</f>
         <v>3858.3500000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+    <row r="29" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="8">
         <v>3859.91</v>
       </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29">
+      <c r="H29">
         <v>3859.35</v>
       </c>
-      <c r="D29">
+      <c r="I29">
         <v>3860.43</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+    <row r="30" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="8">
         <v>3865.53</v>
       </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30">
+      <c r="H30">
         <v>3865.32</v>
       </c>
-      <c r="D30">
+      <c r="I30">
         <v>3865.91</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+    <row r="31" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="10">
         <v>3872.5</v>
       </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31">
+      <c r="H31">
         <v>3872.04</v>
       </c>
-      <c r="D31" s="19">
+      <c r="I31" s="19">
         <v>3872.92</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G32" s="13">
         <v>3882.28</v>
       </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32">
+      <c r="H32">
         <v>3882.1</v>
       </c>
-      <c r="D32">
+      <c r="I32">
         <v>3882.64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G33" s="12">
         <v>3886.28</v>
       </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33">
+      <c r="H33">
         <v>3885.94</v>
       </c>
-      <c r="D33">
+      <c r="I33">
         <v>3886.67</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G34" s="12">
         <v>3887.05</v>
       </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34">
+      <c r="H34">
         <v>3886.79</v>
       </c>
-      <c r="D34">
+      <c r="I34">
         <v>3887.38</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="8">
         <v>3888.52</v>
       </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35">
+      <c r="H35">
         <v>3888.19</v>
       </c>
-      <c r="D35">
+      <c r="I35">
         <v>3889.78</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G36" s="8">
         <v>3895.66</v>
       </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36">
+      <c r="H36">
         <v>3895.33</v>
       </c>
-      <c r="D36">
+      <c r="I36">
         <v>3895.99</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G37" s="8">
         <v>3902.95</v>
       </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37">
+      <c r="H37">
         <v>3902.53</v>
       </c>
-      <c r="D37">
+      <c r="I37">
         <v>3903.56</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G38" s="8">
         <v>3906.45</v>
       </c>
-      <c r="B38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38">
+      <c r="H38">
         <v>3906.14</v>
       </c>
-      <c r="D38">
+      <c r="I38">
         <v>3906.81</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G39" s="8">
         <v>3913.46</v>
       </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39">
+      <c r="H39">
         <v>3913.02</v>
       </c>
-      <c r="D39">
+      <c r="I39">
         <v>3913.98</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G40" s="13">
         <v>3914.48</v>
       </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40">
+      <c r="H40">
         <v>3914.05</v>
       </c>
-      <c r="D40">
+      <c r="I40">
         <v>3914.98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
+    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G41" s="8">
         <v>3920.26</v>
       </c>
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41">
+      <c r="H41">
         <v>3919.98</v>
       </c>
-      <c r="D41">
+      <c r="I41">
         <v>3920.71</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="8">
+    <row r="42" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G42" s="8">
         <v>3922.91</v>
       </c>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42">
+      <c r="H42">
         <v>3922.59</v>
       </c>
-      <c r="D42">
+      <c r="I42">
         <v>3923.4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8">
+    <row r="43" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G43" s="8">
         <v>3927.92</v>
       </c>
-      <c r="B43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43">
+      <c r="H43">
         <v>3927.55</v>
       </c>
-      <c r="D43">
+      <c r="I43">
         <v>3928.4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
+    <row r="44" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G44" s="10">
         <v>3930.3</v>
       </c>
-      <c r="B44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44">
+      <c r="H44">
         <v>3929.47</v>
       </c>
-      <c r="D44">
+      <c r="I44">
         <v>3930.77</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="8">
+    <row r="45" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="8">
         <v>3933.66</v>
       </c>
-      <c r="B45" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45">
-        <f>A45-0.05</f>
+      <c r="H45">
+        <f>G45-0.05</f>
         <v>3933.6099999999997</v>
       </c>
-      <c r="D45">
-        <f>A45+0.05</f>
+      <c r="I45">
+        <f>G45+0.05</f>
         <v>3933.71</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="8">
+    <row r="46" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G46" s="8">
         <v>3938.29</v>
       </c>
-      <c r="B46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46">
+      <c r="H46">
         <v>3938.1</v>
       </c>
-      <c r="D46">
+      <c r="I46">
         <v>3938.83</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="8">
+    <row r="47" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G47" s="8">
         <v>3944.01</v>
       </c>
-      <c r="B47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47">
-        <f>A47-0.05</f>
+      <c r="H47">
+        <f>G47-0.05</f>
         <v>3943.96</v>
       </c>
-      <c r="D47">
-        <f>A47+0.05</f>
+      <c r="I47">
+        <f>G47+0.05</f>
         <v>3944.0600000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="13">
+    <row r="48" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G48" s="13">
         <v>3945.21</v>
       </c>
-      <c r="B48" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48">
-        <f>A48-0.05</f>
+      <c r="H48">
+        <f>G48-0.05</f>
         <v>3945.16</v>
       </c>
-      <c r="D48">
-        <f>A48+0.05</f>
+      <c r="I48">
+        <f>G48+0.05</f>
         <v>3945.26</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="8">
+    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G49" s="8">
         <v>3950.35</v>
       </c>
-      <c r="B49" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49">
-        <f>A49-0.05</f>
+      <c r="H49">
+        <f>G49-0.05</f>
         <v>3950.2999999999997</v>
       </c>
-      <c r="D49">
-        <f>A49+0.05</f>
+      <c r="I49">
+        <f>G49+0.05</f>
         <v>3950.4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="13">
+    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G50" s="13">
         <v>3951.97</v>
       </c>
-      <c r="B50" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50">
-        <f>A50-0.05</f>
+      <c r="H50">
+        <f>G50-0.05</f>
         <v>3951.9199999999996</v>
       </c>
-      <c r="D50">
-        <f>A50+0.05</f>
+      <c r="I50">
+        <f>G50+0.05</f>
         <v>3952.02</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8">
+    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G51" s="8">
         <v>3958.24</v>
       </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51">
-        <f>A51-0.05</f>
+      <c r="H51">
+        <f>G51-0.05</f>
         <v>3958.1899999999996</v>
       </c>
-      <c r="D51">
-        <f>A51+0.05</f>
+      <c r="I51">
+        <f>G51+0.05</f>
         <v>3958.29</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
+    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="8">
         <v>3961.52</v>
       </c>
-      <c r="B52" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52">
-        <f>A52-0.05</f>
+      <c r="H52">
+        <f>G52-0.05</f>
         <v>3961.47</v>
       </c>
-      <c r="D52">
-        <f>A52+0.05</f>
+      <c r="I52">
+        <f>G52+0.05</f>
         <v>3961.57</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="14">
+    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="14">
         <v>3989.8</v>
       </c>
-      <c r="B53" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53">
-        <f>A53-0.05</f>
+      <c r="H53">
+        <f>G53-0.05</f>
         <v>3989.75</v>
       </c>
-      <c r="D53">
-        <f>A53+0.05</f>
+      <c r="I53">
+        <f>G53+0.05</f>
         <v>3989.8500000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="15">
+    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="15">
         <v>3998.98</v>
       </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54">
-        <f t="shared" ref="C54:C55" si="2">A54-0.05</f>
+      <c r="H54">
+        <f>G54-0.05</f>
         <v>3998.93</v>
       </c>
-      <c r="D54">
-        <f t="shared" ref="D54:D55" si="3">A54+0.05</f>
+      <c r="I54">
+        <f>G54+0.05</f>
         <v>3999.03</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="15">
+    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="15">
         <v>4005.71</v>
       </c>
-      <c r="B55" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55">
-        <f t="shared" si="2"/>
+      <c r="H55">
+        <f>G55-0.05</f>
         <v>4005.66</v>
       </c>
-      <c r="D55">
-        <f t="shared" si="3"/>
+      <c r="I55">
+        <f>G55+0.05</f>
         <v>4005.76</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="8">
+    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="8">
         <v>4012.37</v>
       </c>
-      <c r="B56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56">
+      <c r="H56">
         <v>4012.06</v>
       </c>
-      <c r="D56">
+      <c r="I56">
         <v>4012.85</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="8">
+    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="8">
         <v>4028.33</v>
       </c>
-      <c r="B57" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57">
+      <c r="H57">
         <v>4028.09</v>
       </c>
-      <c r="D57">
+      <c r="I57">
         <v>4028.76</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="8">
+    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G58" s="8">
         <v>4030.76</v>
       </c>
-      <c r="B58" t="s">
-        <v>23</v>
-      </c>
-      <c r="C58">
-        <f>A58-0.05</f>
+      <c r="H58">
+        <f>G58-0.05</f>
         <v>4030.71</v>
       </c>
-      <c r="D58">
-        <f>A58+0.05</f>
+      <c r="I58">
+        <f>G58+0.05</f>
         <v>4030.8100000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="8">
+    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="8">
         <v>4033.07</v>
       </c>
-      <c r="B59" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59">
-        <f>A59-0.05</f>
+      <c r="H59">
+        <f>G59-0.05</f>
         <v>4033.02</v>
       </c>
-      <c r="D59">
-        <f>A59+0.05</f>
+      <c r="I59">
+        <f>G59+0.05</f>
         <v>4033.1200000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="8">
+    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="8">
         <v>4034.49</v>
       </c>
-      <c r="B60" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60">
-        <f>A60-0.05</f>
+      <c r="H60">
+        <f>G60-0.05</f>
         <v>4034.4399999999996</v>
       </c>
-      <c r="D60">
-        <f>A60+0.05</f>
+      <c r="I60">
+        <f>G60+0.05</f>
         <v>4034.54</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="8">
+    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="8">
         <v>4035.63</v>
       </c>
-      <c r="B61" t="s">
-        <v>14</v>
-      </c>
-      <c r="C61">
-        <f>A61-0.05</f>
+      <c r="H61">
+        <f>G61-0.05</f>
         <v>4035.58</v>
       </c>
-      <c r="D61">
-        <f>A61+0.05</f>
+      <c r="I61">
+        <f>G61+0.05</f>
         <v>4035.6800000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="8">
+    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="8">
         <v>4045.82</v>
       </c>
-      <c r="B62" t="s">
-        <v>34</v>
-      </c>
-      <c r="C62">
+      <c r="H62">
         <v>4045.41</v>
       </c>
-      <c r="D62">
+      <c r="I62">
         <v>4046.33</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="8">
+    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G63" s="8">
         <v>4063.6</v>
       </c>
-      <c r="B63" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63">
+      <c r="H63">
         <v>4063.12</v>
       </c>
-      <c r="D63">
+      <c r="I63">
         <v>4064.15</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="8">
+    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G64" s="8">
         <v>4071.74</v>
       </c>
-      <c r="B64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C64">
+      <c r="H64">
         <v>4071.39</v>
       </c>
-      <c r="D64" s="19">
+      <c r="I64" s="19">
         <v>4072.17</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="8">
+    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G65" s="8">
         <v>4077.71</v>
       </c>
-      <c r="B65" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65">
+      <c r="H65">
         <v>4173.1499999999996</v>
       </c>
-      <c r="D65">
+      <c r="I65">
         <v>4173.78</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="8">
+    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G66" s="8">
         <v>4101.74</v>
       </c>
-      <c r="B66" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66">
-        <f>A66-0.05</f>
+      <c r="H66">
+        <f>G66-0.05</f>
         <v>4101.6899999999996</v>
       </c>
-      <c r="D66">
-        <f>A66+0.05</f>
+      <c r="I66">
+        <f>G66+0.05</f>
         <v>4101.79</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="8">
+    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G67" s="8">
         <v>4177.54</v>
       </c>
-      <c r="B67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C67">
-        <f>A67-0.05</f>
+      <c r="H67">
+        <f>G67-0.05</f>
         <v>4177.49</v>
       </c>
-      <c r="D67">
-        <f>A67+0.05</f>
+      <c r="I67">
+        <f>G67+0.05</f>
         <v>4177.59</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="8">
+    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G68" s="8">
         <v>4178.8599999999997</v>
       </c>
-      <c r="B68" t="s">
-        <v>35</v>
-      </c>
-      <c r="C68">
+      <c r="H68">
         <v>4178.68</v>
       </c>
-      <c r="D68">
+      <c r="I68">
         <v>4179.2</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="8">
+    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G69" s="8">
         <v>4202.03</v>
       </c>
-      <c r="B69" t="s">
-        <v>34</v>
-      </c>
-      <c r="C69">
+      <c r="H69">
         <v>4201.72</v>
       </c>
-      <c r="D69">
+      <c r="I69">
         <v>4202.51</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="13">
+    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G70" s="13">
         <v>4205.05</v>
       </c>
-      <c r="B70" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70">
-        <f>A70-0.05</f>
+      <c r="H70">
+        <f>G70-0.05</f>
         <v>4205</v>
       </c>
-      <c r="D70">
-        <f>A70+0.05</f>
+      <c r="I70">
+        <f>G70+0.05</f>
         <v>4205.1000000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="8">
+    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G71" s="8">
         <v>4215.5200000000004</v>
       </c>
-      <c r="B71" t="s">
-        <v>25</v>
-      </c>
-      <c r="C71">
-        <f>A71-0.05</f>
+      <c r="H71">
+        <f>G71-0.05</f>
         <v>4215.47</v>
       </c>
-      <c r="D71">
-        <f>A71+0.05</f>
+      <c r="I71">
+        <f>G71+0.05</f>
         <v>4215.5700000000006</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="8">
+    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G72" s="8">
         <v>4226.7299999999996</v>
       </c>
-      <c r="B72" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72">
-        <f>A72-0.05</f>
+      <c r="H72">
+        <f>G72-0.05</f>
         <v>4226.6799999999994</v>
       </c>
-      <c r="D72">
-        <f>A72+0.05</f>
+      <c r="I72">
+        <f>G72+0.05</f>
         <v>4226.78</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="8">
+    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G73" s="8">
         <v>4233.16</v>
       </c>
-      <c r="B73" t="s">
-        <v>35</v>
-      </c>
-      <c r="C73">
+      <c r="H73">
         <v>4232.49</v>
       </c>
-      <c r="D73">
+      <c r="I73">
         <v>4233.82</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
+    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G74" s="8">
         <v>4246.83</v>
       </c>
-      <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74">
-        <f>A74-0.05</f>
+      <c r="H74">
+        <f>G74-0.05</f>
         <v>4246.78</v>
       </c>
-      <c r="D74">
-        <f>A74+0.05</f>
+      <c r="I74">
+        <f>G74+0.05</f>
         <v>4246.88</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="8">
+    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G75" s="8">
         <v>4250.79</v>
       </c>
-      <c r="B75" t="s">
-        <v>34</v>
-      </c>
-      <c r="C75">
+      <c r="H75">
         <v>4250.43</v>
       </c>
-      <c r="D75">
+      <c r="I75">
         <v>4251.26</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G76" s="8">
         <v>4254.3500000000004</v>
       </c>
-      <c r="B76" t="s">
-        <v>28</v>
-      </c>
-      <c r="C76">
-        <f>A76-0.05</f>
+      <c r="H76">
+        <f>G76-0.05</f>
         <v>4254.3</v>
       </c>
-      <c r="D76">
-        <f>A76+0.05</f>
+      <c r="I76">
+        <f>G76+0.05</f>
         <v>4254.4000000000005</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="13">
+    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G77" s="13">
         <v>4258.16</v>
       </c>
-      <c r="B77" t="s">
-        <v>35</v>
-      </c>
-      <c r="C77">
+      <c r="H77">
         <v>4257.87</v>
       </c>
-      <c r="D77">
+      <c r="I77">
         <v>4258.75</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
+    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G78" s="8">
         <v>4271.76</v>
       </c>
-      <c r="B78" t="s">
-        <v>34</v>
-      </c>
-      <c r="C78">
+      <c r="H78">
         <v>4271.3900000000003</v>
       </c>
-      <c r="D78">
+      <c r="I78">
         <v>4272.1899999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
+    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G79" s="8">
         <v>4274.8</v>
       </c>
-      <c r="B79" t="s">
-        <v>28</v>
-      </c>
-      <c r="C79">
-        <f>A79-0.05</f>
+      <c r="H79">
+        <f>G79-0.05</f>
         <v>4274.75</v>
       </c>
-      <c r="D79">
-        <f>A79+0.05</f>
+      <c r="I79">
+        <f>G79+0.05</f>
         <v>4274.8500000000004</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="8">
+    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G80" s="8">
         <v>4294.1000000000004</v>
       </c>
-      <c r="B80" t="s">
-        <v>36</v>
-      </c>
-      <c r="C80">
+      <c r="H80">
         <v>4293.4799999999996</v>
       </c>
-      <c r="D80">
+      <c r="I80">
         <v>4294.5200000000004</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="8">
+    <row r="81" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G81" s="8">
         <v>4300.05</v>
       </c>
-      <c r="B81" t="s">
-        <v>36</v>
-      </c>
-      <c r="C81">
+      <c r="H81">
         <v>4299.75</v>
       </c>
-      <c r="D81">
+      <c r="I81">
         <v>4300.8100000000004</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="8">
+    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G82" s="8">
         <v>4307.8999999999996</v>
       </c>
-      <c r="B82" t="s">
-        <v>36</v>
-      </c>
-      <c r="C82">
+      <c r="H82">
         <v>430.75099999999998</v>
       </c>
-      <c r="D82">
+      <c r="I82">
         <v>4308.43</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="8">
+    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G83" s="8">
         <v>4312.8599999999997</v>
       </c>
-      <c r="B83" t="s">
-        <v>36</v>
-      </c>
-      <c r="C83">
+      <c r="H83">
         <v>4312.6099999999997</v>
       </c>
-      <c r="D83">
+      <c r="I83">
         <v>4313.29</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="8">
+    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G84" s="8">
         <v>4320.75</v>
       </c>
-      <c r="B84" t="s">
-        <v>9</v>
-      </c>
-      <c r="C84">
-        <f>A84-0.05</f>
+      <c r="H84">
+        <f>G84-0.05</f>
         <v>4320.7</v>
       </c>
-      <c r="D84">
-        <f>A84+0.05</f>
+      <c r="I84">
+        <f>G84+0.05</f>
         <v>4320.8</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="8">
+    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G85" s="8">
         <v>4320.75</v>
       </c>
-      <c r="B85" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85">
-        <f>A85-0.05</f>
+      <c r="H85">
+        <f>G85-0.05</f>
         <v>4320.7</v>
       </c>
-      <c r="D85">
-        <f>A85+0.05</f>
+      <c r="I85">
+        <f>G85+0.05</f>
         <v>4320.8</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="8">
+    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G86" s="8">
         <v>4340.47</v>
       </c>
-      <c r="B86" t="s">
-        <v>29</v>
-      </c>
-      <c r="C86">
-        <f>A86-0.05</f>
+      <c r="H86">
+        <f>G86-0.05</f>
         <v>4340.42</v>
       </c>
-      <c r="D86">
-        <f>A86+0.05</f>
+      <c r="I86">
+        <f>G86+0.05</f>
         <v>4340.5200000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="13">
+    <row r="87" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G87" s="13">
         <v>4344.29</v>
       </c>
-      <c r="B87" t="s">
-        <v>36</v>
-      </c>
-      <c r="C87">
+      <c r="H87">
         <v>4344.07</v>
       </c>
-      <c r="D87">
+      <c r="I87">
         <v>4344.7299999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="8">
+    <row r="88" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G88" s="8">
         <v>4351.76</v>
       </c>
-      <c r="B88" t="s">
-        <v>35</v>
-      </c>
-      <c r="C88">
+      <c r="H88">
         <v>4351.3900000000003</v>
       </c>
-      <c r="D88">
+      <c r="I88">
         <v>4352.29</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="8">
+    <row r="89" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G89" s="8">
         <v>4383.55</v>
       </c>
-      <c r="B89" t="s">
-        <v>34</v>
-      </c>
-      <c r="C89">
+      <c r="H89">
         <v>4383.1499999999996</v>
       </c>
-      <c r="D89">
+      <c r="I89">
         <v>4384.04</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="8">
+    <row r="90" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G90" s="8">
         <v>4395.03</v>
       </c>
-      <c r="B90" t="s">
-        <v>36</v>
-      </c>
-      <c r="C90">
+      <c r="H90">
         <v>4394.66</v>
       </c>
-      <c r="D90">
+      <c r="I90">
         <v>4395.63</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="8">
+    <row r="91" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G91" s="8">
         <v>4399.7700000000004</v>
       </c>
-      <c r="B91" t="s">
-        <v>36</v>
-      </c>
-      <c r="C91">
+      <c r="H91">
         <v>4399.4799999999996</v>
       </c>
-      <c r="D91">
+      <c r="I91">
         <v>4400.0720000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="8">
+    <row r="92" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G92" s="8">
         <v>4400.3599999999997</v>
       </c>
-      <c r="B92" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92">
-        <f>A92-0.05</f>
+      <c r="H92">
+        <f>G92-0.05</f>
         <v>4400.3099999999995</v>
       </c>
-      <c r="D92">
-        <f>A92+0.05</f>
+      <c r="I92">
+        <f>G92+0.05</f>
         <v>4400.41</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="8">
+    <row r="93" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G93" s="8">
         <v>4404.75</v>
       </c>
-      <c r="B93" t="s">
-        <v>34</v>
-      </c>
-      <c r="C93">
+      <c r="H93">
         <v>4404.3999999999996</v>
       </c>
-      <c r="D93">
+      <c r="I93">
         <v>4405.25</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="13">
+    <row r="94" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G94" s="13">
         <v>4417.72</v>
       </c>
-      <c r="B94" t="s">
-        <v>36</v>
-      </c>
-      <c r="C94">
+      <c r="H94">
         <v>4417.46</v>
       </c>
-      <c r="D94">
+      <c r="I94">
         <v>4418</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="10">
+    <row r="95" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G95" s="10">
         <v>4443.8</v>
       </c>
-      <c r="B95" t="s">
-        <v>36</v>
-      </c>
-      <c r="C95">
+      <c r="H95">
         <v>4443.4799999999996</v>
       </c>
-      <c r="D95">
+      <c r="I95">
         <v>4444.46</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="8">
+    <row r="96" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G96" s="8">
         <v>4468.49</v>
       </c>
-      <c r="B96" t="s">
-        <v>36</v>
-      </c>
-      <c r="C96">
+      <c r="H96">
         <v>4468.1400000000003</v>
       </c>
-      <c r="D96">
+      <c r="I96">
         <v>4468.97</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="8">
+    <row r="97" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G97" s="8">
         <v>4501.2700000000004</v>
       </c>
-      <c r="B97" t="s">
-        <v>36</v>
-      </c>
-      <c r="C97">
+      <c r="H97">
         <v>4500.88</v>
       </c>
-      <c r="D97">
+      <c r="I97">
         <v>4501.67</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="8">
+    <row r="98" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G98" s="8">
         <v>4522.63</v>
       </c>
-      <c r="B98" t="s">
-        <v>35</v>
-      </c>
-      <c r="C98">
+      <c r="H98">
         <v>4522.24</v>
       </c>
-      <c r="D98">
+      <c r="I98">
         <v>4523.16</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="8">
+    <row r="99" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G99" s="8">
         <v>4533.97</v>
       </c>
-      <c r="B99" t="s">
-        <v>36</v>
-      </c>
-      <c r="C99">
+      <c r="H99">
         <v>4533.6499999999996</v>
       </c>
-      <c r="D99">
+      <c r="I99">
         <v>4534.4399999999996</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="8">
+    <row r="100" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G100" s="8">
         <v>4549.62</v>
       </c>
-      <c r="B100" t="s">
-        <v>36</v>
-      </c>
-      <c r="C100">
+      <c r="H100">
         <v>4549.0600000000004</v>
       </c>
-      <c r="D100">
+      <c r="I100">
         <v>4550.08</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="8">
+    <row r="101" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G101" s="8">
         <v>4554.03</v>
       </c>
-      <c r="B101" t="s">
-        <v>30</v>
-      </c>
-      <c r="C101">
-        <f>A101-0.05</f>
+      <c r="H101">
+        <f>G101-0.05</f>
         <v>4553.9799999999996</v>
       </c>
-      <c r="D101">
-        <f>A101+0.05</f>
+      <c r="I101">
+        <f>G101+0.05</f>
         <v>4554.08</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="8">
+    <row r="102" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G102" s="8">
         <v>4563.76</v>
       </c>
-      <c r="B102" t="s">
-        <v>36</v>
-      </c>
-      <c r="C102">
+      <c r="H102">
         <v>4563.4799999999996</v>
       </c>
-      <c r="D102">
+      <c r="I102">
         <v>4564.32</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="8">
+    <row r="103" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G103" s="8">
         <v>4571.97</v>
       </c>
-      <c r="B103" t="s">
-        <v>36</v>
-      </c>
-      <c r="C103">
+      <c r="H103">
         <v>4571.47</v>
       </c>
-      <c r="D103">
+      <c r="I103">
         <v>4572.4799999999996</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="8">
+    <row r="104" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G104" s="8">
         <v>4583.83</v>
       </c>
-      <c r="B104" t="s">
-        <v>35</v>
-      </c>
-      <c r="C104">
+      <c r="H104">
         <v>4583.03</v>
       </c>
-      <c r="D104">
+      <c r="I104">
         <v>4583.5200000000004</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="13">
+    <row r="105" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G105" s="13">
         <v>4589.96</v>
       </c>
-      <c r="B105" t="s">
-        <v>36</v>
-      </c>
-      <c r="C105">
+      <c r="H105">
         <v>4589.62</v>
       </c>
-      <c r="D105">
+      <c r="I105">
         <v>4590.28</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="13">
+    <row r="106" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G106" s="13">
         <v>4629.34</v>
       </c>
-      <c r="B106" t="s">
-        <v>35</v>
-      </c>
-      <c r="C106">
+      <c r="H106">
         <v>4629.1000000000004</v>
       </c>
-      <c r="D106">
+      <c r="I106">
         <v>4629.6899999999996</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pruebas con espectro puro y substracted: ancho eq y ewr
</commit_message>
<xml_diff>
--- a/Scripts/Growth_curve/lines.xlsx
+++ b/Scripts/Growth_curve/lines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucia\Documents\Semestre8y9\Trabajo_grado\Tesis_Estrellas_binarias\Scripts\Growth_curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DF2FCC-B88E-4468-B0F9-EA66A6CC1FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0EDF7-0C6D-47E0-9707-007340CE4DDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="1000" activeTab="3" xr2:uid="{F6AB02B0-D3FC-4D31-BBAC-19215CAECE6C}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="36">
   <si>
     <t>wavelenght</t>
   </si>
@@ -130,7 +130,13 @@
     <t>*</t>
   </si>
   <si>
-    <t>wave_peak</t>
+    <t>waveobs</t>
+  </si>
+  <si>
+    <t>Fe 1</t>
+  </si>
+  <si>
+    <t>Ti 2</t>
   </si>
 </sst>
 </file>
@@ -10595,1258 +10601,1576 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE75F030-7D08-4563-BE0C-CE0E8301EC84}">
-  <dimension ref="G1:I106"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G2" s="8">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>3761.32</v>
       </c>
-      <c r="H2">
+      <c r="B2">
         <v>3760.75</v>
       </c>
-      <c r="I2">
+      <c r="C2">
         <v>3762.1</v>
       </c>
-    </row>
-    <row r="3" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G3" s="8">
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>3763.79</v>
       </c>
-      <c r="H3">
+      <c r="B3">
         <v>3763.4</v>
       </c>
-      <c r="I3">
+      <c r="C3">
         <v>3764.34</v>
       </c>
-    </row>
-    <row r="4" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G4" s="8">
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>3767.19</v>
       </c>
-      <c r="H4">
+      <c r="B4">
         <v>3766.7</v>
       </c>
-      <c r="I4">
+      <c r="C4">
         <v>3767.55</v>
       </c>
-    </row>
-    <row r="5" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G5" s="8">
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>3769.46</v>
       </c>
-      <c r="H5">
-        <f>G5-0.05</f>
+      <c r="B5">
+        <f>A5-0.05</f>
         <v>3769.41</v>
       </c>
-      <c r="I5">
-        <f>G5+0.05</f>
+      <c r="C5">
+        <f>A5+0.05</f>
         <v>3769.51</v>
       </c>
-    </row>
-    <row r="6" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G6" s="8">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>3770.63</v>
       </c>
-      <c r="H6">
-        <f>G6-0.05</f>
+      <c r="B6">
+        <f>A6-0.05</f>
         <v>3770.58</v>
       </c>
-      <c r="I6">
-        <f>G6+0.05</f>
+      <c r="C6">
+        <f>A6+0.05</f>
         <v>3770.6800000000003</v>
       </c>
-    </row>
-    <row r="7" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="8">
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>3774.33</v>
       </c>
-      <c r="H7">
-        <f>G7-0.05</f>
+      <c r="B7">
+        <f>A7-0.05</f>
         <v>3774.2799999999997</v>
       </c>
-      <c r="I7">
-        <f>G7+0.05</f>
+      <c r="C7">
+        <f>A7+0.05</f>
         <v>3774.38</v>
       </c>
-    </row>
-    <row r="8" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="8">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>3783.35</v>
       </c>
-      <c r="H8">
+      <c r="B8">
         <v>3783.25</v>
       </c>
-      <c r="I8">
+      <c r="C8">
         <v>3783.75</v>
       </c>
-    </row>
-    <row r="9" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G9" s="8">
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>3787.88</v>
       </c>
-      <c r="H9">
+      <c r="B9">
         <v>3787.58</v>
       </c>
-      <c r="I9">
+      <c r="C9">
         <v>3788.21</v>
       </c>
-    </row>
-    <row r="10" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G10" s="8">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>3788.7</v>
       </c>
-      <c r="H10">
-        <f>G10-0.05</f>
+      <c r="B10">
+        <f>A10-0.05</f>
         <v>3788.6499999999996</v>
       </c>
-      <c r="I10">
-        <f>G10+0.05</f>
+      <c r="C10">
+        <f>A10+0.05</f>
         <v>3788.75</v>
       </c>
-    </row>
-    <row r="11" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G11" s="10">
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>3795</v>
       </c>
-      <c r="H11">
+      <c r="B11">
         <v>3794.58</v>
       </c>
-      <c r="I11">
+      <c r="C11">
         <v>3795.38</v>
       </c>
-    </row>
-    <row r="12" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="8">
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <v>3797.9</v>
       </c>
-      <c r="H12">
-        <f>G12-0.05</f>
+      <c r="B12">
+        <f>A12-0.05</f>
         <v>3797.85</v>
       </c>
-      <c r="I12">
-        <f>G12+0.05</f>
+      <c r="C12">
+        <f>A12+0.05</f>
         <v>3797.9500000000003</v>
       </c>
-    </row>
-    <row r="13" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G13" s="8">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>3814.58</v>
       </c>
-      <c r="H13">
+      <c r="B13">
         <v>3814.18</v>
       </c>
-      <c r="I13">
+      <c r="C13">
         <v>3815.1</v>
       </c>
-    </row>
-    <row r="14" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="8">
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <v>3815.84</v>
       </c>
-      <c r="H14">
+      <c r="B14">
         <v>3815.5</v>
       </c>
-      <c r="I14">
+      <c r="C14">
         <v>3816.3</v>
       </c>
-    </row>
-    <row r="15" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="8">
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>3820.43</v>
       </c>
-      <c r="H15" s="18">
+      <c r="B15" s="18">
         <v>3819.98</v>
       </c>
-      <c r="I15">
+      <c r="C15">
         <v>3821.02</v>
       </c>
-    </row>
-    <row r="16" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="8">
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
         <v>3824.45</v>
       </c>
-      <c r="H16">
+      <c r="B16">
         <v>3824.05</v>
       </c>
-      <c r="I16">
+      <c r="C16">
         <v>3824.91</v>
       </c>
-    </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G17" s="8">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>3825.88</v>
       </c>
-      <c r="H17">
+      <c r="B17">
         <v>3825.5</v>
       </c>
-      <c r="I17">
+      <c r="C17">
         <v>3826.46</v>
       </c>
-    </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="8">
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <v>3827.83</v>
       </c>
-      <c r="H18">
+      <c r="B18">
         <v>3827.43</v>
       </c>
-      <c r="I18">
+      <c r="C18">
         <v>3828.23</v>
       </c>
-    </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="8">
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
         <v>3829.35</v>
       </c>
-      <c r="H19">
-        <f>G19-0.05</f>
+      <c r="B19">
+        <f>A19-0.05</f>
         <v>3829.2999999999997</v>
       </c>
-      <c r="I19">
-        <f>G19+0.05</f>
+      <c r="C19">
+        <f>A19+0.05</f>
         <v>3829.4</v>
       </c>
-    </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G20" s="8">
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <v>3832.3</v>
       </c>
-      <c r="H20">
-        <f>G20-0.05</f>
+      <c r="B20">
+        <f>A20-0.05</f>
         <v>3832.25</v>
       </c>
-      <c r="I20">
-        <f>G20+0.05</f>
+      <c r="C20">
+        <f>A20+0.05</f>
         <v>3832.3500000000004</v>
       </c>
-    </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G21" s="8">
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
         <v>3834.23</v>
       </c>
-      <c r="H21">
+      <c r="B21">
         <v>3833.77</v>
       </c>
-      <c r="I21">
+      <c r="C21">
         <v>3834.69</v>
       </c>
-    </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="8">
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
         <v>3835.39</v>
       </c>
-      <c r="H22">
-        <f>G22-0.05</f>
+      <c r="B22">
+        <f>A22-0.05</f>
         <v>3835.3399999999997</v>
       </c>
-      <c r="I22">
-        <f>G22+0.05</f>
+      <c r="C22">
+        <f>A22+0.05</f>
         <v>3835.44</v>
       </c>
-    </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="8">
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
         <v>3838.29</v>
       </c>
-      <c r="H23">
-        <f>G23-0.05</f>
+      <c r="B23">
+        <f>A23-0.05</f>
         <v>3838.24</v>
       </c>
-      <c r="I23">
-        <f>G23+0.05</f>
+      <c r="C23">
+        <f>A23+0.05</f>
         <v>3838.34</v>
       </c>
-    </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="8">
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
         <v>3843.03</v>
       </c>
-      <c r="H24">
-        <f>G24-0.05</f>
+      <c r="B24">
+        <f>A24-0.05</f>
         <v>3842.98</v>
       </c>
-      <c r="I24">
-        <f>G24+0.05</f>
+      <c r="C24">
+        <f>A24+0.05</f>
         <v>3843.0800000000004</v>
       </c>
-    </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="10">
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
         <v>3850</v>
       </c>
-      <c r="H25">
+      <c r="B25">
         <v>3849.65</v>
       </c>
-      <c r="I25">
+      <c r="C25">
         <v>3850.3</v>
       </c>
-    </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="8">
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
         <v>3850.82</v>
       </c>
-      <c r="H26">
+      <c r="B26">
         <v>3850.55</v>
       </c>
-      <c r="I26">
+      <c r="C26">
         <v>3851.15</v>
       </c>
-    </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G27" s="8">
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
         <v>3856.37</v>
       </c>
-      <c r="H27">
+      <c r="B27">
         <v>3855.97</v>
       </c>
-      <c r="I27">
+      <c r="C27">
         <v>3856.85</v>
       </c>
-    </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G28" s="8">
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
         <v>3858.3</v>
       </c>
-      <c r="H28">
-        <f>G28-0.05</f>
+      <c r="B28">
+        <f>A28-0.05</f>
         <v>3858.25</v>
       </c>
-      <c r="I28">
-        <f>G28+0.05</f>
+      <c r="C28">
+        <f>A28+0.05</f>
         <v>3858.3500000000004</v>
       </c>
-    </row>
-    <row r="29" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="8">
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
         <v>3859.91</v>
       </c>
-      <c r="H29">
+      <c r="B29">
         <v>3859.35</v>
       </c>
-      <c r="I29">
+      <c r="C29">
         <v>3860.43</v>
       </c>
-    </row>
-    <row r="30" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="8">
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
         <v>3865.53</v>
       </c>
-      <c r="H30">
+      <c r="B30">
         <v>3865.32</v>
       </c>
-      <c r="I30">
+      <c r="C30">
         <v>3865.91</v>
       </c>
-    </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="10">
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
         <v>3872.5</v>
       </c>
-      <c r="H31">
+      <c r="B31">
         <v>3872.04</v>
       </c>
-      <c r="I31" s="19">
+      <c r="C31" s="19">
         <v>3872.92</v>
       </c>
-    </row>
-    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G32" s="13">
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
         <v>3882.28</v>
       </c>
-      <c r="H32">
+      <c r="B32">
         <v>3882.1</v>
       </c>
-      <c r="I32">
+      <c r="C32">
         <v>3882.64</v>
       </c>
-    </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G33" s="12">
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
         <v>3886.28</v>
       </c>
-      <c r="H33">
+      <c r="B33">
         <v>3885.94</v>
       </c>
-      <c r="I33">
+      <c r="C33">
         <v>3886.67</v>
       </c>
-    </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G34" s="12">
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
         <v>3887.05</v>
       </c>
-      <c r="H34">
+      <c r="B34">
         <v>3886.79</v>
       </c>
-      <c r="I34">
+      <c r="C34">
         <v>3887.38</v>
       </c>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G35" s="8">
+      <c r="D34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
         <v>3888.52</v>
       </c>
-      <c r="H35">
+      <c r="B35">
         <v>3888.19</v>
       </c>
-      <c r="I35">
+      <c r="C35">
         <v>3889.78</v>
       </c>
-    </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G36" s="8">
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
         <v>3895.66</v>
       </c>
-      <c r="H36">
+      <c r="B36">
         <v>3895.33</v>
       </c>
-      <c r="I36">
+      <c r="C36">
         <v>3895.99</v>
       </c>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G37" s="8">
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
         <v>3902.95</v>
       </c>
-      <c r="H37">
+      <c r="B37">
         <v>3902.53</v>
       </c>
-      <c r="I37">
+      <c r="C37">
         <v>3903.56</v>
       </c>
-    </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G38" s="8">
+      <c r="D37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
         <v>3906.45</v>
       </c>
-      <c r="H38">
+      <c r="B38">
         <v>3906.14</v>
       </c>
-      <c r="I38">
+      <c r="C38">
         <v>3906.81</v>
       </c>
-    </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G39" s="8">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
         <v>3913.46</v>
       </c>
-      <c r="H39">
+      <c r="B39">
         <v>3913.02</v>
       </c>
-      <c r="I39">
+      <c r="C39">
         <v>3913.98</v>
       </c>
-    </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G40" s="13">
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
         <v>3914.48</v>
       </c>
-      <c r="H40">
+      <c r="B40">
         <v>3914.05</v>
       </c>
-      <c r="I40">
+      <c r="C40">
         <v>3914.98</v>
       </c>
-    </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G41" s="8">
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
         <v>3920.26</v>
       </c>
-      <c r="H41">
+      <c r="B41">
         <v>3919.98</v>
       </c>
-      <c r="I41">
+      <c r="C41">
         <v>3920.71</v>
       </c>
-    </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G42" s="8">
+      <c r="D41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
         <v>3922.91</v>
       </c>
-      <c r="H42">
+      <c r="B42">
         <v>3922.59</v>
       </c>
-      <c r="I42">
+      <c r="C42">
         <v>3923.4</v>
       </c>
-    </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G43" s="8">
+      <c r="D42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
         <v>3927.92</v>
       </c>
-      <c r="H43">
+      <c r="B43">
         <v>3927.55</v>
       </c>
-      <c r="I43">
+      <c r="C43">
         <v>3928.4</v>
       </c>
-    </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G44" s="10">
+      <c r="D43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
         <v>3930.3</v>
       </c>
-      <c r="H44">
+      <c r="B44">
         <v>3929.47</v>
       </c>
-      <c r="I44">
+      <c r="C44">
         <v>3930.77</v>
       </c>
-    </row>
-    <row r="45" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G45" s="8">
+      <c r="D44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
         <v>3933.66</v>
       </c>
-      <c r="H45">
-        <f>G45-0.05</f>
+      <c r="B45">
+        <f>A45-0.05</f>
         <v>3933.6099999999997</v>
       </c>
-      <c r="I45">
-        <f>G45+0.05</f>
+      <c r="C45">
+        <f>A45+0.05</f>
         <v>3933.71</v>
       </c>
-    </row>
-    <row r="46" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G46" s="8">
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
         <v>3938.29</v>
       </c>
-      <c r="H46">
+      <c r="B46">
         <v>3938.1</v>
       </c>
-      <c r="I46">
+      <c r="C46">
         <v>3938.83</v>
       </c>
-    </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G47" s="8">
+      <c r="D46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
         <v>3944.01</v>
       </c>
-      <c r="H47">
-        <f>G47-0.05</f>
+      <c r="B47">
+        <f t="shared" ref="B47:B55" si="0">A47-0.05</f>
         <v>3943.96</v>
       </c>
-      <c r="I47">
-        <f>G47+0.05</f>
+      <c r="C47">
+        <f t="shared" ref="C47:C55" si="1">A47+0.05</f>
         <v>3944.0600000000004</v>
       </c>
-    </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G48" s="13">
+      <c r="D47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
         <v>3945.21</v>
       </c>
-      <c r="H48">
-        <f>G48-0.05</f>
+      <c r="B48">
+        <f t="shared" si="0"/>
         <v>3945.16</v>
       </c>
-      <c r="I48">
-        <f>G48+0.05</f>
+      <c r="C48">
+        <f t="shared" si="1"/>
         <v>3945.26</v>
       </c>
-    </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="8">
+      <c r="D48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
         <v>3950.35</v>
       </c>
-      <c r="H49">
-        <f>G49-0.05</f>
+      <c r="B49">
+        <f t="shared" si="0"/>
         <v>3950.2999999999997</v>
       </c>
-      <c r="I49">
-        <f>G49+0.05</f>
+      <c r="C49">
+        <f t="shared" si="1"/>
         <v>3950.4</v>
       </c>
-    </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G50" s="13">
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
         <v>3951.97</v>
       </c>
-      <c r="H50">
-        <f>G50-0.05</f>
+      <c r="B50">
+        <f t="shared" si="0"/>
         <v>3951.9199999999996</v>
       </c>
-      <c r="I50">
-        <f>G50+0.05</f>
+      <c r="C50">
+        <f t="shared" si="1"/>
         <v>3952.02</v>
       </c>
-    </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="8">
+      <c r="D50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
         <v>3958.24</v>
       </c>
-      <c r="H51">
-        <f>G51-0.05</f>
+      <c r="B51">
+        <f t="shared" si="0"/>
         <v>3958.1899999999996</v>
       </c>
-      <c r="I51">
-        <f>G51+0.05</f>
+      <c r="C51">
+        <f t="shared" si="1"/>
         <v>3958.29</v>
       </c>
-    </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="8">
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
         <v>3961.52</v>
       </c>
-      <c r="H52">
-        <f>G52-0.05</f>
+      <c r="B52">
+        <f t="shared" si="0"/>
         <v>3961.47</v>
       </c>
-      <c r="I52">
-        <f>G52+0.05</f>
+      <c r="C52">
+        <f t="shared" si="1"/>
         <v>3961.57</v>
       </c>
-    </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="14">
+      <c r="D52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
         <v>3989.8</v>
       </c>
-      <c r="H53">
-        <f>G53-0.05</f>
+      <c r="B53">
+        <f t="shared" si="0"/>
         <v>3989.75</v>
       </c>
-      <c r="I53">
-        <f>G53+0.05</f>
+      <c r="C53">
+        <f t="shared" si="1"/>
         <v>3989.8500000000004</v>
       </c>
-    </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="15">
+      <c r="D53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
         <v>3998.98</v>
       </c>
-      <c r="H54">
-        <f>G54-0.05</f>
+      <c r="B54">
+        <f t="shared" si="0"/>
         <v>3998.93</v>
       </c>
-      <c r="I54">
-        <f>G54+0.05</f>
+      <c r="C54">
+        <f t="shared" si="1"/>
         <v>3999.03</v>
       </c>
-    </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="15">
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
         <v>4005.71</v>
       </c>
-      <c r="H55">
-        <f>G55-0.05</f>
+      <c r="B55">
+        <f t="shared" si="0"/>
         <v>4005.66</v>
       </c>
-      <c r="I55">
-        <f>G55+0.05</f>
+      <c r="C55">
+        <f t="shared" si="1"/>
         <v>4005.76</v>
       </c>
-    </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="8">
+      <c r="D55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
         <v>4012.37</v>
       </c>
-      <c r="H56">
+      <c r="B56">
         <v>4012.06</v>
       </c>
-      <c r="I56">
+      <c r="C56">
         <v>4012.85</v>
       </c>
-    </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G57" s="8">
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
         <v>4028.33</v>
       </c>
-      <c r="H57">
+      <c r="B57">
         <v>4028.09</v>
       </c>
-      <c r="I57">
+      <c r="C57">
         <v>4028.76</v>
       </c>
-    </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G58" s="8">
+      <c r="D57" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
         <v>4030.76</v>
       </c>
-      <c r="H58">
-        <f>G58-0.05</f>
+      <c r="B58">
+        <f>A58-0.05</f>
         <v>4030.71</v>
       </c>
-      <c r="I58">
-        <f>G58+0.05</f>
+      <c r="C58">
+        <f>A58+0.05</f>
         <v>4030.8100000000004</v>
       </c>
-    </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G59" s="8">
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
         <v>4033.07</v>
       </c>
-      <c r="H59">
-        <f>G59-0.05</f>
+      <c r="B59">
+        <f>A59-0.05</f>
         <v>4033.02</v>
       </c>
-      <c r="I59">
-        <f>G59+0.05</f>
+      <c r="C59">
+        <f>A59+0.05</f>
         <v>4033.1200000000003</v>
       </c>
-    </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G60" s="8">
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
         <v>4034.49</v>
       </c>
-      <c r="H60">
-        <f>G60-0.05</f>
+      <c r="B60">
+        <f>A60-0.05</f>
         <v>4034.4399999999996</v>
       </c>
-      <c r="I60">
-        <f>G60+0.05</f>
+      <c r="C60">
+        <f>A60+0.05</f>
         <v>4034.54</v>
       </c>
-    </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G61" s="8">
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
         <v>4035.63</v>
       </c>
-      <c r="H61">
-        <f>G61-0.05</f>
+      <c r="B61">
+        <f>A61-0.05</f>
         <v>4035.58</v>
       </c>
-      <c r="I61">
-        <f>G61+0.05</f>
+      <c r="C61">
+        <f>A61+0.05</f>
         <v>4035.6800000000003</v>
       </c>
-    </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G62" s="8">
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
         <v>4045.82</v>
       </c>
-      <c r="H62">
+      <c r="B62">
         <v>4045.41</v>
       </c>
-      <c r="I62">
+      <c r="C62">
         <v>4046.33</v>
       </c>
-    </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G63" s="8">
+      <c r="D62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="8">
         <v>4063.6</v>
       </c>
-      <c r="H63">
+      <c r="B63">
         <v>4063.12</v>
       </c>
-      <c r="I63">
+      <c r="C63">
         <v>4064.15</v>
       </c>
-    </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G64" s="8">
+      <c r="D63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
         <v>4071.74</v>
       </c>
-      <c r="H64">
+      <c r="B64">
         <v>4071.39</v>
       </c>
-      <c r="I64" s="19">
+      <c r="C64" s="19">
         <v>4072.17</v>
       </c>
-    </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G65" s="8">
+      <c r="D64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="8">
         <v>4077.71</v>
       </c>
-      <c r="H65">
+      <c r="B65">
         <v>4173.1499999999996</v>
       </c>
-      <c r="I65">
+      <c r="C65">
         <v>4173.78</v>
       </c>
-    </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G66" s="8">
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
         <v>4101.74</v>
       </c>
-      <c r="H66">
-        <f>G66-0.05</f>
+      <c r="B66">
+        <f>A66-0.05</f>
         <v>4101.6899999999996</v>
       </c>
-      <c r="I66">
-        <f>G66+0.05</f>
+      <c r="C66">
+        <f>A66+0.05</f>
         <v>4101.79</v>
       </c>
-    </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G67" s="8">
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="8">
         <v>4177.54</v>
       </c>
-      <c r="H67">
-        <f>G67-0.05</f>
+      <c r="B67">
+        <f>A67-0.05</f>
         <v>4177.49</v>
       </c>
-      <c r="I67">
-        <f>G67+0.05</f>
+      <c r="C67">
+        <f>A67+0.05</f>
         <v>4177.59</v>
       </c>
-    </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G68" s="8">
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
         <v>4178.8599999999997</v>
       </c>
-      <c r="H68">
+      <c r="B68">
         <v>4178.68</v>
       </c>
-      <c r="I68">
+      <c r="C68">
         <v>4179.2</v>
       </c>
-    </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G69" s="8">
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="8">
         <v>4202.03</v>
       </c>
-      <c r="H69">
+      <c r="B69">
         <v>4201.72</v>
       </c>
-      <c r="I69">
+      <c r="C69">
         <v>4202.51</v>
       </c>
-    </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G70" s="13">
+      <c r="D69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="13">
         <v>4205.05</v>
       </c>
-      <c r="H70">
-        <f>G70-0.05</f>
+      <c r="B70">
+        <f>A70-0.05</f>
         <v>4205</v>
       </c>
-      <c r="I70">
-        <f>G70+0.05</f>
+      <c r="C70">
+        <f>A70+0.05</f>
         <v>4205.1000000000004</v>
       </c>
-    </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G71" s="8">
+      <c r="D70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
         <v>4215.5200000000004</v>
       </c>
-      <c r="H71">
-        <f>G71-0.05</f>
+      <c r="B71">
+        <f>A71-0.05</f>
         <v>4215.47</v>
       </c>
-      <c r="I71">
-        <f>G71+0.05</f>
+      <c r="C71">
+        <f>A71+0.05</f>
         <v>4215.5700000000006</v>
       </c>
-    </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G72" s="8">
+      <c r="D71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="8">
         <v>4226.7299999999996</v>
       </c>
-      <c r="H72">
-        <f>G72-0.05</f>
+      <c r="B72">
+        <f>A72-0.05</f>
         <v>4226.6799999999994</v>
       </c>
-      <c r="I72">
-        <f>G72+0.05</f>
+      <c r="C72">
+        <f>A72+0.05</f>
         <v>4226.78</v>
       </c>
-    </row>
-    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G73" s="8">
+      <c r="D72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="8">
         <v>4233.16</v>
       </c>
-      <c r="H73">
+      <c r="B73">
         <v>4232.49</v>
       </c>
-      <c r="I73">
+      <c r="C73">
         <v>4233.82</v>
       </c>
-    </row>
-    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G74" s="8">
+      <c r="D73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="8">
         <v>4246.83</v>
       </c>
-      <c r="H74">
-        <f>G74-0.05</f>
+      <c r="B74">
+        <f>A74-0.05</f>
         <v>4246.78</v>
       </c>
-      <c r="I74">
-        <f>G74+0.05</f>
+      <c r="C74">
+        <f>A74+0.05</f>
         <v>4246.88</v>
       </c>
-    </row>
-    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G75" s="8">
+      <c r="D74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="8">
         <v>4250.79</v>
       </c>
-      <c r="H75">
+      <c r="B75">
         <v>4250.43</v>
       </c>
-      <c r="I75">
+      <c r="C75">
         <v>4251.26</v>
       </c>
-    </row>
-    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G76" s="8">
+      <c r="D75" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="8">
         <v>4254.3500000000004</v>
       </c>
-      <c r="H76">
-        <f>G76-0.05</f>
+      <c r="B76">
+        <f>A76-0.05</f>
         <v>4254.3</v>
       </c>
-      <c r="I76">
-        <f>G76+0.05</f>
+      <c r="C76">
+        <f>A76+0.05</f>
         <v>4254.4000000000005</v>
       </c>
-    </row>
-    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G77" s="13">
+      <c r="D76" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="13">
         <v>4258.16</v>
       </c>
-      <c r="H77">
+      <c r="B77">
         <v>4257.87</v>
       </c>
-      <c r="I77">
+      <c r="C77">
         <v>4258.75</v>
       </c>
-    </row>
-    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G78" s="8">
+      <c r="D77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="8">
         <v>4271.76</v>
       </c>
-      <c r="H78">
+      <c r="B78">
         <v>4271.3900000000003</v>
       </c>
-      <c r="I78">
+      <c r="C78">
         <v>4272.1899999999996</v>
       </c>
-    </row>
-    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G79" s="8">
+      <c r="D78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="8">
         <v>4274.8</v>
       </c>
-      <c r="H79">
-        <f>G79-0.05</f>
+      <c r="B79">
+        <f>A79-0.05</f>
         <v>4274.75</v>
       </c>
-      <c r="I79">
-        <f>G79+0.05</f>
+      <c r="C79">
+        <f>A79+0.05</f>
         <v>4274.8500000000004</v>
       </c>
-    </row>
-    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G80" s="8">
+      <c r="D79" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="8">
         <v>4294.1000000000004</v>
       </c>
-      <c r="H80">
+      <c r="B80">
         <v>4293.4799999999996</v>
       </c>
-      <c r="I80">
+      <c r="C80">
         <v>4294.5200000000004</v>
       </c>
-    </row>
-    <row r="81" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G81" s="8">
+      <c r="D80" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="8">
         <v>4300.05</v>
       </c>
-      <c r="H81">
+      <c r="B81">
         <v>4299.75</v>
       </c>
-      <c r="I81">
+      <c r="C81">
         <v>4300.8100000000004</v>
       </c>
-    </row>
-    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G82" s="8">
+      <c r="D81" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="8">
         <v>4307.8999999999996</v>
       </c>
-      <c r="H82">
+      <c r="B82">
         <v>430.75099999999998</v>
       </c>
-      <c r="I82">
+      <c r="C82">
         <v>4308.43</v>
       </c>
-    </row>
-    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G83" s="8">
+      <c r="D82" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="8">
         <v>4312.8599999999997</v>
       </c>
-      <c r="H83">
+      <c r="B83">
         <v>4312.6099999999997</v>
       </c>
-      <c r="I83">
+      <c r="C83">
         <v>4313.29</v>
       </c>
-    </row>
-    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G84" s="8">
+      <c r="D83" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="8">
         <v>4320.75</v>
       </c>
-      <c r="H84">
-        <f>G84-0.05</f>
+      <c r="B84">
+        <f>A84-0.05</f>
         <v>4320.7</v>
       </c>
-      <c r="I84">
-        <f>G84+0.05</f>
+      <c r="C84">
+        <f>A84+0.05</f>
         <v>4320.8</v>
       </c>
-    </row>
-    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G85" s="8">
+      <c r="D84" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="8">
         <v>4320.75</v>
       </c>
-      <c r="H85">
-        <f>G85-0.05</f>
+      <c r="B85">
+        <f>A85-0.05</f>
         <v>4320.7</v>
       </c>
-      <c r="I85">
-        <f>G85+0.05</f>
+      <c r="C85">
+        <f>A85+0.05</f>
         <v>4320.8</v>
       </c>
-    </row>
-    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G86" s="8">
+      <c r="D85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="8">
         <v>4340.47</v>
       </c>
-      <c r="H86">
-        <f>G86-0.05</f>
+      <c r="B86">
+        <f>A86-0.05</f>
         <v>4340.42</v>
       </c>
-      <c r="I86">
-        <f>G86+0.05</f>
+      <c r="C86">
+        <f>A86+0.05</f>
         <v>4340.5200000000004</v>
       </c>
-    </row>
-    <row r="87" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G87" s="13">
+      <c r="D86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="13">
         <v>4344.29</v>
       </c>
-      <c r="H87">
+      <c r="B87">
         <v>4344.07</v>
       </c>
-      <c r="I87">
+      <c r="C87">
         <v>4344.7299999999996</v>
       </c>
-    </row>
-    <row r="88" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G88" s="8">
+      <c r="D87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
         <v>4351.76</v>
       </c>
-      <c r="H88">
+      <c r="B88">
         <v>4351.3900000000003</v>
       </c>
-      <c r="I88">
+      <c r="C88">
         <v>4352.29</v>
       </c>
-    </row>
-    <row r="89" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G89" s="8">
+      <c r="D88" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="8">
         <v>4383.55</v>
       </c>
-      <c r="H89">
+      <c r="B89">
         <v>4383.1499999999996</v>
       </c>
-      <c r="I89">
+      <c r="C89">
         <v>4384.04</v>
       </c>
-    </row>
-    <row r="90" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G90" s="8">
+      <c r="D89" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="8">
         <v>4395.03</v>
       </c>
-      <c r="H90">
+      <c r="B90">
         <v>4394.66</v>
       </c>
-      <c r="I90">
+      <c r="C90">
         <v>4395.63</v>
       </c>
-    </row>
-    <row r="91" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G91" s="8">
+      <c r="D90" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="8">
         <v>4399.7700000000004</v>
       </c>
-      <c r="H91">
+      <c r="B91">
         <v>4399.4799999999996</v>
       </c>
-      <c r="I91">
+      <c r="C91">
         <v>4400.0720000000001</v>
       </c>
-    </row>
-    <row r="92" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G92" s="8">
+      <c r="D91" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="8">
         <v>4400.3599999999997</v>
       </c>
-      <c r="H92">
-        <f>G92-0.05</f>
+      <c r="B92">
+        <f>A92-0.05</f>
         <v>4400.3099999999995</v>
       </c>
-      <c r="I92">
-        <f>G92+0.05</f>
+      <c r="C92">
+        <f>A92+0.05</f>
         <v>4400.41</v>
       </c>
-    </row>
-    <row r="93" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G93" s="8">
+      <c r="D92" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="8">
         <v>4404.75</v>
       </c>
-      <c r="H93">
+      <c r="B93">
         <v>4404.3999999999996</v>
       </c>
-      <c r="I93">
+      <c r="C93">
         <v>4405.25</v>
       </c>
-    </row>
-    <row r="94" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G94" s="13">
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="13">
         <v>4417.72</v>
       </c>
-      <c r="H94">
+      <c r="B94">
         <v>4417.46</v>
       </c>
-      <c r="I94">
+      <c r="C94">
         <v>4418</v>
       </c>
-    </row>
-    <row r="95" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G95" s="10">
+      <c r="D94" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="10">
         <v>4443.8</v>
       </c>
-      <c r="H95">
+      <c r="B95">
         <v>4443.4799999999996</v>
       </c>
-      <c r="I95">
+      <c r="C95">
         <v>4444.46</v>
       </c>
-    </row>
-    <row r="96" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G96" s="8">
+      <c r="D95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="8">
         <v>4468.49</v>
       </c>
-      <c r="H96">
+      <c r="B96">
         <v>4468.1400000000003</v>
       </c>
-      <c r="I96">
+      <c r="C96">
         <v>4468.97</v>
       </c>
-    </row>
-    <row r="97" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G97" s="8">
+      <c r="D96" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="8">
         <v>4501.2700000000004</v>
       </c>
-      <c r="H97">
+      <c r="B97">
         <v>4500.88</v>
       </c>
-      <c r="I97">
+      <c r="C97">
         <v>4501.67</v>
       </c>
-    </row>
-    <row r="98" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G98" s="8">
+      <c r="D97" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="8">
         <v>4522.63</v>
       </c>
-      <c r="H98">
+      <c r="B98">
         <v>4522.24</v>
       </c>
-      <c r="I98">
+      <c r="C98">
         <v>4523.16</v>
       </c>
-    </row>
-    <row r="99" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G99" s="8">
+      <c r="D98" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="8">
         <v>4533.97</v>
       </c>
-      <c r="H99">
+      <c r="B99">
         <v>4533.6499999999996</v>
       </c>
-      <c r="I99">
+      <c r="C99">
         <v>4534.4399999999996</v>
       </c>
-    </row>
-    <row r="100" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G100" s="8">
+      <c r="D99" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="8">
         <v>4549.62</v>
       </c>
-      <c r="H100">
+      <c r="B100">
         <v>4549.0600000000004</v>
       </c>
-      <c r="I100">
+      <c r="C100">
         <v>4550.08</v>
       </c>
-    </row>
-    <row r="101" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G101" s="8">
+      <c r="D100" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="8">
         <v>4554.03</v>
       </c>
-      <c r="H101">
-        <f>G101-0.05</f>
+      <c r="B101">
+        <f>A101-0.05</f>
         <v>4553.9799999999996</v>
       </c>
-      <c r="I101">
-        <f>G101+0.05</f>
+      <c r="C101">
+        <f>A101+0.05</f>
         <v>4554.08</v>
       </c>
-    </row>
-    <row r="102" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G102" s="8">
+      <c r="D101" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="8">
         <v>4563.76</v>
       </c>
-      <c r="H102">
+      <c r="B102">
         <v>4563.4799999999996</v>
       </c>
-      <c r="I102">
+      <c r="C102">
         <v>4564.32</v>
       </c>
-    </row>
-    <row r="103" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G103" s="8">
+      <c r="D102" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="8">
         <v>4571.97</v>
       </c>
-      <c r="H103">
+      <c r="B103">
         <v>4571.47</v>
       </c>
-      <c r="I103">
+      <c r="C103">
         <v>4572.4799999999996</v>
       </c>
-    </row>
-    <row r="104" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G104" s="8">
+      <c r="D103" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="8">
         <v>4583.83</v>
       </c>
-      <c r="H104">
+      <c r="B104">
         <v>4583.03</v>
       </c>
-      <c r="I104">
+      <c r="C104">
         <v>4583.5200000000004</v>
       </c>
-    </row>
-    <row r="105" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G105" s="13">
+      <c r="D104" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="13">
         <v>4589.96</v>
       </c>
-      <c r="H105">
+      <c r="B105">
         <v>4589.62</v>
       </c>
-      <c r="I105">
+      <c r="C105">
         <v>4590.28</v>
       </c>
-    </row>
-    <row r="106" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G106" s="13">
+      <c r="D105" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="13">
         <v>4629.34</v>
       </c>
-      <c r="H106">
+      <c r="B106">
         <v>4629.1000000000004</v>
       </c>
-      <c r="I106">
+      <c r="C106">
         <v>4629.6899999999996</v>
+      </c>
+      <c r="D106" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>